<commit_message>
One last bug remaining to be entered.
</commit_message>
<xml_diff>
--- a/data/mother_laying_bydate.xlsx
+++ b/data/mother_laying_bydate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/git_repositories/extreme-flight-trials/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C54D1B-875E-AD4C-BAEA-226C38FCAD67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DEB235-E84A-5C4D-BCD4-81D6122B16F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="500" windowWidth="28040" windowHeight="16640" xr2:uid="{E14F8870-8DED-064C-A3A0-F7635F8AECA1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="15">
   <si>
     <t>collect_date</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>10.29.21</t>
+  </si>
+  <si>
+    <t>11.01.21</t>
+  </si>
+  <si>
+    <t>11.02.21</t>
+  </si>
+  <si>
+    <t>11.05.21</t>
   </si>
 </sst>
 </file>
@@ -412,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EE6B1BE-B14C-BE4C-BCD4-C1716963499F}">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A175" sqref="A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1529,6 +1538,15 @@
       <c r="B66" t="s">
         <v>11</v>
       </c>
+      <c r="C66">
+        <v>8</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67">
@@ -1537,6 +1555,15 @@
       <c r="B67" t="s">
         <v>11</v>
       </c>
+      <c r="C67">
+        <v>27</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68">
@@ -1545,6 +1572,15 @@
       <c r="B68" t="s">
         <v>11</v>
       </c>
+      <c r="C68">
+        <v>66</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+      <c r="E68" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
@@ -1553,30 +1589,1799 @@
       <c r="B69" t="s">
         <v>11</v>
       </c>
+      <c r="C69">
+        <v>11</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1113</v>
       </c>
+      <c r="B70" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70">
+        <v>10</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1274</v>
       </c>
+      <c r="B71" t="s">
+        <v>11</v>
+      </c>
+      <c r="C71">
+        <v>18</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1291</v>
       </c>
+      <c r="B72" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72">
+        <v>45</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1225</v>
       </c>
+      <c r="B73" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73">
+        <v>42</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1353</v>
+      </c>
+      <c r="B74" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74">
+        <v>15</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>1244</v>
+      </c>
+      <c r="B75" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75">
+        <v>8</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>1296</v>
+      </c>
+      <c r="B76" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76">
+        <v>48</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>1235</v>
+      </c>
+      <c r="B77" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>1049</v>
+      </c>
+      <c r="B78" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78">
+        <v>6</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>1314</v>
+      </c>
+      <c r="B79" t="s">
+        <v>11</v>
+      </c>
+      <c r="C79">
+        <v>98</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>1017</v>
+      </c>
+      <c r="B80" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80">
+        <v>3</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>1016</v>
+      </c>
+      <c r="B81" t="s">
+        <v>11</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>1288</v>
+      </c>
+      <c r="B82" t="s">
+        <v>11</v>
+      </c>
+      <c r="C82">
+        <v>41</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>1255</v>
+      </c>
+      <c r="B83" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83">
+        <v>43</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>1111</v>
+      </c>
+      <c r="B84" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84">
+        <v>16</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>1212</v>
+      </c>
+      <c r="B85" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85">
+        <v>33</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>1123</v>
+      </c>
+      <c r="B86" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86">
+        <v>5</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>1058</v>
+      </c>
+      <c r="B87" t="s">
+        <v>11</v>
+      </c>
+      <c r="C87">
+        <v>12</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>1233</v>
+      </c>
+      <c r="B88" t="s">
+        <v>11</v>
+      </c>
+      <c r="C88">
+        <v>10</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>1105</v>
+      </c>
+      <c r="B89" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89">
+        <v>23</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+      <c r="E89" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>1507</v>
+      </c>
+      <c r="B90" t="s">
+        <v>11</v>
+      </c>
+      <c r="C90">
+        <v>17</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>1289</v>
+      </c>
+      <c r="B91" t="s">
+        <v>11</v>
+      </c>
+      <c r="C91">
+        <v>13</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+      <c r="E91" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>1013</v>
+      </c>
+      <c r="B92" t="s">
+        <v>11</v>
+      </c>
+      <c r="C92">
+        <v>58</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>1356</v>
+      </c>
+      <c r="B93" t="s">
+        <v>11</v>
+      </c>
+      <c r="C93">
+        <v>8</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>1566.5</v>
+      </c>
+      <c r="B94" t="s">
+        <v>11</v>
+      </c>
+      <c r="C94">
+        <v>8</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>1055</v>
+      </c>
+      <c r="B95" t="s">
+        <v>11</v>
+      </c>
+      <c r="C95">
+        <v>27</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>1121</v>
+      </c>
+      <c r="B96" t="s">
+        <v>11</v>
+      </c>
+      <c r="C96">
+        <v>5</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>1206</v>
+      </c>
+      <c r="B97" t="s">
+        <v>11</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>1011</v>
+      </c>
+      <c r="B98" t="s">
+        <v>11</v>
+      </c>
+      <c r="C98">
+        <v>49</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>1064</v>
+      </c>
+      <c r="B99" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99">
+        <v>5</v>
+      </c>
+      <c r="D99">
+        <v>0</v>
+      </c>
+      <c r="E99" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>1161</v>
+      </c>
+      <c r="B100" t="s">
+        <v>12</v>
+      </c>
+      <c r="C100">
+        <v>16</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>1680</v>
+      </c>
+      <c r="B101" t="s">
+        <v>12</v>
+      </c>
+      <c r="C101">
+        <v>40</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>1145</v>
+      </c>
+      <c r="B102" t="s">
+        <v>12</v>
+      </c>
+      <c r="C102">
+        <v>27</v>
+      </c>
+      <c r="D102">
+        <v>0</v>
+      </c>
+      <c r="E102" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>1030</v>
+      </c>
+      <c r="B103" t="s">
+        <v>12</v>
+      </c>
+      <c r="C103">
+        <v>35</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>1538</v>
+      </c>
+      <c r="B104" t="s">
+        <v>12</v>
+      </c>
+      <c r="C104">
+        <v>26</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>1655</v>
+      </c>
+      <c r="B105" t="s">
+        <v>12</v>
+      </c>
+      <c r="C105">
+        <v>51</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>1168</v>
+      </c>
+      <c r="B106" t="s">
+        <v>12</v>
+      </c>
+      <c r="C106">
+        <v>12</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>1383</v>
+      </c>
+      <c r="B107" t="s">
+        <v>12</v>
+      </c>
+      <c r="C107">
+        <v>44</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>1141</v>
+      </c>
+      <c r="B108" t="s">
+        <v>12</v>
+      </c>
+      <c r="C108">
+        <v>16</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>1421</v>
+      </c>
+      <c r="B109" t="s">
+        <v>12</v>
+      </c>
+      <c r="C109">
+        <v>3</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+      <c r="E109" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>1607</v>
+      </c>
+      <c r="B110" t="s">
+        <v>12</v>
+      </c>
+      <c r="C110">
+        <v>21</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+      <c r="E110" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>1469</v>
+      </c>
+      <c r="B111" t="s">
+        <v>12</v>
+      </c>
+      <c r="C111">
+        <v>15</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+      <c r="E111" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>1203</v>
+      </c>
+      <c r="B112" t="s">
+        <v>12</v>
+      </c>
+      <c r="C112">
+        <v>22</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>1609</v>
+      </c>
+      <c r="B113" t="s">
+        <v>12</v>
+      </c>
+      <c r="C113">
+        <v>34</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>1546</v>
+      </c>
+      <c r="B114" t="s">
+        <v>12</v>
+      </c>
+      <c r="C114">
+        <v>16</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>1437</v>
+      </c>
+      <c r="B115" t="s">
+        <v>12</v>
+      </c>
+      <c r="C115">
+        <v>39</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>1169</v>
+      </c>
+      <c r="B116" t="s">
+        <v>12</v>
+      </c>
+      <c r="C116">
+        <v>4</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>1495</v>
+      </c>
+      <c r="B117" t="s">
+        <v>12</v>
+      </c>
+      <c r="C117">
+        <v>63</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+      <c r="E117" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>1139</v>
+      </c>
+      <c r="B118" t="s">
+        <v>12</v>
+      </c>
+      <c r="C118">
+        <v>17</v>
+      </c>
+      <c r="D118">
+        <v>0</v>
+      </c>
+      <c r="E118" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>1395</v>
+      </c>
+      <c r="B119" t="s">
+        <v>12</v>
+      </c>
+      <c r="C119">
+        <v>13</v>
+      </c>
+      <c r="D119">
+        <v>0</v>
+      </c>
+      <c r="E119" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>1616</v>
+      </c>
+      <c r="B120" t="s">
+        <v>12</v>
+      </c>
+      <c r="C120">
+        <v>56</v>
+      </c>
+      <c r="D120">
+        <v>0</v>
+      </c>
+      <c r="E120" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>1026</v>
+      </c>
+      <c r="B121" t="s">
+        <v>12</v>
+      </c>
+      <c r="C121">
+        <v>3</v>
+      </c>
+      <c r="D121">
+        <v>0</v>
+      </c>
+      <c r="E121" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>1401</v>
+      </c>
+      <c r="B122" t="s">
+        <v>12</v>
+      </c>
+      <c r="C122">
+        <v>10</v>
+      </c>
+      <c r="D122">
+        <v>0</v>
+      </c>
+      <c r="E122" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>1734</v>
+      </c>
+      <c r="B123" t="s">
+        <v>12</v>
+      </c>
+      <c r="C123">
+        <v>22</v>
+      </c>
+      <c r="D123">
+        <v>0</v>
+      </c>
+      <c r="E123" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>1461</v>
+      </c>
+      <c r="B124" t="s">
+        <v>12</v>
+      </c>
+      <c r="C124">
+        <v>10</v>
+      </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+      <c r="E124" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>1548</v>
+      </c>
+      <c r="B125" t="s">
+        <v>12</v>
+      </c>
+      <c r="C125">
+        <v>29</v>
+      </c>
+      <c r="D125">
+        <v>0</v>
+      </c>
+      <c r="E125" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>1587</v>
+      </c>
+      <c r="B126" t="s">
+        <v>12</v>
+      </c>
+      <c r="C126">
+        <v>15</v>
+      </c>
+      <c r="D126">
+        <v>0</v>
+      </c>
+      <c r="E126" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>1531</v>
+      </c>
+      <c r="B127" t="s">
+        <v>12</v>
+      </c>
+      <c r="C127">
+        <v>8</v>
+      </c>
+      <c r="D127">
+        <v>0</v>
+      </c>
+      <c r="E127" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>1682</v>
+      </c>
+      <c r="B128" t="s">
+        <v>12</v>
+      </c>
+      <c r="C128">
+        <v>46</v>
+      </c>
+      <c r="D128">
+        <v>0</v>
+      </c>
+      <c r="E128" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>1459</v>
+      </c>
+      <c r="B129" t="s">
+        <v>12</v>
+      </c>
+      <c r="C129">
+        <v>41</v>
+      </c>
+      <c r="D129">
+        <v>0</v>
+      </c>
+      <c r="E129" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>1123</v>
+      </c>
+      <c r="B130" t="s">
+        <v>13</v>
+      </c>
+      <c r="C130">
+        <v>5</v>
+      </c>
+      <c r="D130">
+        <v>0</v>
+      </c>
+      <c r="E130" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>1288</v>
+      </c>
+      <c r="B131" t="s">
+        <v>13</v>
+      </c>
+      <c r="C131">
+        <v>18</v>
+      </c>
+      <c r="D131">
+        <v>0</v>
+      </c>
+      <c r="E131" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>1291</v>
+      </c>
+      <c r="B132" t="s">
+        <v>13</v>
+      </c>
+      <c r="C132">
+        <v>5</v>
+      </c>
+      <c r="D132">
+        <v>0</v>
+      </c>
+      <c r="E132" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>1353</v>
+      </c>
+      <c r="B133" t="s">
+        <v>13</v>
+      </c>
+      <c r="C133">
+        <v>27</v>
+      </c>
+      <c r="D133">
+        <v>0</v>
+      </c>
+      <c r="E133" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>1269</v>
+      </c>
+      <c r="B134" t="s">
+        <v>13</v>
+      </c>
+      <c r="C134">
+        <v>25</v>
+      </c>
+      <c r="D134">
+        <v>0</v>
+      </c>
+      <c r="E134" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>1356</v>
+      </c>
+      <c r="B135" t="s">
+        <v>13</v>
+      </c>
+      <c r="C135">
+        <v>11</v>
+      </c>
+      <c r="D135">
+        <v>0</v>
+      </c>
+      <c r="E135" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>1016</v>
+      </c>
+      <c r="B136" t="s">
+        <v>13</v>
+      </c>
+      <c r="C136">
+        <v>2</v>
+      </c>
+      <c r="D136">
+        <v>0</v>
+      </c>
+      <c r="E136" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>1255</v>
+      </c>
+      <c r="B137" t="s">
+        <v>13</v>
+      </c>
+      <c r="C137">
+        <v>17</v>
+      </c>
+      <c r="D137">
+        <v>0</v>
+      </c>
+      <c r="E137" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>1055</v>
+      </c>
+      <c r="B138" t="s">
+        <v>13</v>
+      </c>
+      <c r="C138">
+        <v>2</v>
+      </c>
+      <c r="D138">
+        <v>0</v>
+      </c>
+      <c r="E138" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>1064</v>
+      </c>
+      <c r="B139" t="s">
+        <v>13</v>
+      </c>
+      <c r="C139">
+        <v>11</v>
+      </c>
+      <c r="D139">
+        <v>0</v>
+      </c>
+      <c r="E139" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>1314</v>
+      </c>
+      <c r="B140" t="s">
+        <v>13</v>
+      </c>
+      <c r="C140">
+        <v>5</v>
+      </c>
+      <c r="D140">
+        <v>0</v>
+      </c>
+      <c r="E140" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>1046</v>
+      </c>
+      <c r="B141" t="s">
+        <v>13</v>
+      </c>
+      <c r="C141">
+        <v>2</v>
+      </c>
+      <c r="D141">
+        <v>0</v>
+      </c>
+      <c r="E141" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>1296</v>
+      </c>
+      <c r="B142" t="s">
+        <v>13</v>
+      </c>
+      <c r="C142">
+        <v>26</v>
+      </c>
+      <c r="D142">
+        <v>0</v>
+      </c>
+      <c r="E142" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>1274</v>
+      </c>
+      <c r="B143" t="s">
+        <v>13</v>
+      </c>
+      <c r="C143">
+        <v>3</v>
+      </c>
+      <c r="D143">
+        <v>0</v>
+      </c>
+      <c r="E143" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>1584</v>
+      </c>
+      <c r="B144" t="s">
+        <v>13</v>
+      </c>
+      <c r="C144">
+        <v>26</v>
+      </c>
+      <c r="D144">
+        <v>0</v>
+      </c>
+      <c r="E144" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>1735</v>
+      </c>
+      <c r="B145" t="s">
+        <v>13</v>
+      </c>
+      <c r="C145">
+        <v>9</v>
+      </c>
+      <c r="D145">
+        <v>0</v>
+      </c>
+      <c r="E145" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>1686</v>
+      </c>
+      <c r="B146" t="s">
+        <v>13</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
+      </c>
+      <c r="D146">
+        <v>0</v>
+      </c>
+      <c r="E146" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>1121</v>
+      </c>
+      <c r="B147" t="s">
+        <v>13</v>
+      </c>
+      <c r="C147">
+        <v>2</v>
+      </c>
+      <c r="D147">
+        <v>0</v>
+      </c>
+      <c r="E147" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>1544</v>
+      </c>
+      <c r="B148" t="s">
+        <v>13</v>
+      </c>
+      <c r="C148">
+        <v>6</v>
+      </c>
+      <c r="D148">
+        <v>0</v>
+      </c>
+      <c r="E148" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>1225</v>
+      </c>
+      <c r="B149" t="s">
+        <v>13</v>
+      </c>
+      <c r="C149">
+        <v>6</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+      <c r="E149" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>1233</v>
+      </c>
+      <c r="B150" t="s">
+        <v>13</v>
+      </c>
+      <c r="C150">
+        <v>9</v>
+      </c>
+      <c r="D150">
+        <v>0</v>
+      </c>
+      <c r="E150" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>1013</v>
+      </c>
+      <c r="B151" t="s">
+        <v>13</v>
+      </c>
+      <c r="C151">
+        <v>16</v>
+      </c>
+      <c r="D151">
+        <v>0</v>
+      </c>
+      <c r="E151" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>1206</v>
+      </c>
+      <c r="B152" t="s">
+        <v>13</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
+      </c>
+      <c r="D152">
+        <v>0</v>
+      </c>
+      <c r="E152" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>1113</v>
+      </c>
+      <c r="B153" t="s">
+        <v>13</v>
+      </c>
+      <c r="C153">
+        <v>5</v>
+      </c>
+      <c r="D153">
+        <v>0</v>
+      </c>
+      <c r="E153" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>1111</v>
+      </c>
+      <c r="B154" t="s">
+        <v>13</v>
+      </c>
+      <c r="C154">
+        <v>4</v>
+      </c>
+      <c r="D154">
+        <v>0</v>
+      </c>
+      <c r="E154" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>1105</v>
+      </c>
+      <c r="B155" t="s">
+        <v>13</v>
+      </c>
+      <c r="C155">
+        <v>6</v>
+      </c>
+      <c r="D155">
+        <v>0</v>
+      </c>
+      <c r="E155" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>1244</v>
+      </c>
+      <c r="B156" t="s">
+        <v>13</v>
+      </c>
+      <c r="C156">
+        <v>7</v>
+      </c>
+      <c r="D156">
+        <v>0</v>
+      </c>
+      <c r="E156" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>1570</v>
+      </c>
+      <c r="B157" t="s">
+        <v>13</v>
+      </c>
+      <c r="C157">
+        <v>9</v>
+      </c>
+      <c r="D157">
+        <v>0</v>
+      </c>
+      <c r="E157" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>1212</v>
+      </c>
+      <c r="B158" t="s">
+        <v>13</v>
+      </c>
+      <c r="C158">
+        <v>3</v>
+      </c>
+      <c r="D158">
+        <v>0</v>
+      </c>
+      <c r="E158" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>1235</v>
+      </c>
+      <c r="B159" t="s">
+        <v>13</v>
+      </c>
+      <c r="C159">
+        <v>1</v>
+      </c>
+      <c r="D159">
+        <v>0</v>
+      </c>
+      <c r="E159" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>1011</v>
+      </c>
+      <c r="B160" t="s">
+        <v>13</v>
+      </c>
+      <c r="C160">
+        <v>33</v>
+      </c>
+      <c r="D160">
+        <v>0</v>
+      </c>
+      <c r="E160" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>1214</v>
+      </c>
+      <c r="B161" t="s">
+        <v>13</v>
+      </c>
+      <c r="C161">
+        <v>9</v>
+      </c>
+      <c r="D161">
+        <v>0</v>
+      </c>
+      <c r="E161" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>1208</v>
+      </c>
+      <c r="B162" t="s">
+        <v>13</v>
+      </c>
+      <c r="C162">
+        <v>1</v>
+      </c>
+      <c r="D162">
+        <v>0</v>
+      </c>
+      <c r="E162" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>1741</v>
+      </c>
+      <c r="B163" t="s">
+        <v>14</v>
+      </c>
+      <c r="C163">
+        <v>8</v>
+      </c>
+      <c r="D163">
+        <v>0</v>
+      </c>
+      <c r="E163" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>1736</v>
+      </c>
+      <c r="B164" t="s">
+        <v>14</v>
+      </c>
+      <c r="C164">
+        <v>10</v>
+      </c>
+      <c r="D164">
+        <v>0</v>
+      </c>
+      <c r="E164" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>1687</v>
+      </c>
+      <c r="B165" t="s">
+        <v>14</v>
+      </c>
+      <c r="C165">
+        <v>4</v>
+      </c>
+      <c r="D165">
+        <v>0</v>
+      </c>
+      <c r="E165" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>1536</v>
+      </c>
+      <c r="B166" t="s">
+        <v>14</v>
+      </c>
+      <c r="C166">
+        <v>3</v>
+      </c>
+      <c r="D166">
+        <v>0</v>
+      </c>
+      <c r="E166" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>1329</v>
+      </c>
+      <c r="B167" t="s">
+        <v>14</v>
+      </c>
+      <c r="C167">
+        <v>7</v>
+      </c>
+      <c r="D167">
+        <v>0</v>
+      </c>
+      <c r="E167" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>1612</v>
+      </c>
+      <c r="B168" t="s">
+        <v>14</v>
+      </c>
+      <c r="C168">
+        <v>6</v>
+      </c>
+      <c r="D168">
+        <v>0</v>
+      </c>
+      <c r="E168" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>1627</v>
+      </c>
+      <c r="B169" t="s">
+        <v>14</v>
+      </c>
+      <c r="C169">
+        <v>27</v>
+      </c>
+      <c r="D169">
+        <v>0</v>
+      </c>
+      <c r="E169" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>1729</v>
+      </c>
+      <c r="B170" t="s">
+        <v>14</v>
+      </c>
+      <c r="C170">
+        <v>28</v>
+      </c>
+      <c r="D170">
+        <v>0</v>
+      </c>
+      <c r="E170" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>1739</v>
+      </c>
+      <c r="B171" t="s">
+        <v>14</v>
+      </c>
+      <c r="C171">
+        <v>18</v>
+      </c>
+      <c r="D171">
+        <v>0</v>
+      </c>
+      <c r="E171" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>1738</v>
+      </c>
+      <c r="B172" t="s">
+        <v>14</v>
+      </c>
+      <c r="C172">
+        <v>38</v>
+      </c>
+      <c r="D172">
+        <v>0</v>
+      </c>
+      <c r="E172" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>1542</v>
+      </c>
+      <c r="B173" t="s">
+        <v>14</v>
+      </c>
+      <c r="C173">
+        <v>17</v>
+      </c>
+      <c r="D173">
+        <v>0</v>
+      </c>
+      <c r="E173" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>1743</v>
+      </c>
+      <c r="B174" t="s">
+        <v>14</v>
+      </c>
+      <c r="C174">
+        <v>4</v>
+      </c>
+      <c r="D174">
+        <v>0</v>
+      </c>
+      <c r="E174" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>